<commit_message>
Refaktorisan Ugovor kontroler i dodat izmjenjeni dnevnik za it54
</commit_message>
<xml_diff>
--- a/SonarCloud/IT54-2018_Milan_Brčkalo.xlsx
+++ b/SonarCloud/IT54-2018_Milan_Brčkalo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="63">
   <si>
     <t>Upravljanje razvojem informacionih sistema</t>
   </si>
@@ -320,6 +320,21 @@
     <t>Class changed to static type</t>
   </si>
   <si>
+    <t>S107</t>
+  </si>
+  <si>
+    <t>Should be moved in another class</t>
+  </si>
+  <si>
+    <t>Added helper class</t>
+  </si>
+  <si>
+    <t>Disagree</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t xml:space="preserve">Percieved criticality </t>
   </si>
   <si>
@@ -365,9 +380,6 @@
     <t>Undecided</t>
   </si>
   <si>
-    <t>Disagree</t>
-  </si>
-  <si>
     <t>Very easy</t>
   </si>
   <si>
@@ -378,9 +390,6 @@
   </si>
   <si>
     <t>Decission on refactoring</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Useful to the given issue</t>
@@ -1714,32 +1723,80 @@
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
+      <c r="A22" s="19">
+        <v>44614.0</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="20">
+        <v>10.0</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
+      <c r="A23" s="19">
+        <v>44615.0</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="20">
+        <v>10.0</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="21"/>
@@ -4558,15 +4615,15 @@
     <row r="2" ht="14.25" customHeight="1"/>
     <row r="3" ht="14.25" customHeight="1">
       <c r="B3" s="25" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="B4" s="26" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>17</v>
@@ -4577,7 +4634,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
@@ -4590,18 +4647,18 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="B7" s="27" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="B8" s="28" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1"/>
@@ -4609,23 +4666,23 @@
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1">
       <c r="B12" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="B13" s="26" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="B14" s="27" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>22</v>
@@ -4633,10 +4690,10 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="B15" s="27" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -4644,30 +4701,30 @@
         <v>20</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="B17" s="28" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1">
       <c r="B20" s="25" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="B21" s="26" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G21" s="26" t="s">
         <v>18</v>
@@ -4678,25 +4735,25 @@
         <v>22</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="B23" s="27" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="B24" s="27" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="B25" s="28" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -4706,7 +4763,7 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="G27" s="28" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1"/>

</xml_diff>